<commit_message>
up to 8 code
</commit_message>
<xml_diff>
--- a/CODES.xlsx
+++ b/CODES.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F92B293-B379-473B-8B72-CB9FD3FB4AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E176DC-6A9C-4D68-9ECB-A2E56244A47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="855" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
   <si>
     <t>HS Code</t>
   </si>
@@ -204,6 +204,129 @@
   </si>
   <si>
     <t>16041400</t>
+  </si>
+  <si>
+    <t>Tunas</t>
+  </si>
+  <si>
+    <t>Chewing gum</t>
+  </si>
+  <si>
+    <t>Sugar confectionery other than chewing gum</t>
+  </si>
+  <si>
+    <t>Chocolate &amp; other food preparations containing cocoa</t>
+  </si>
+  <si>
+    <t>Prepared foods obt. by the swelling/roasting of cereals/cereal products</t>
+  </si>
+  <si>
+    <t>Sweet biscuits</t>
+  </si>
+  <si>
+    <t>Waffles &amp; wafers</t>
+  </si>
+  <si>
+    <t>Bread, pastry, cakes, biscuits &amp; other bakers' wares, whether</t>
+  </si>
+  <si>
+    <t>Vegetables, fruit, nuts by vinegar</t>
+  </si>
+  <si>
+    <t>Cucumbers &amp; gherkins, prepared  by vinegar</t>
+  </si>
+  <si>
+    <t>Tomatoes othw. than by vinegar in pieces</t>
+  </si>
+  <si>
+    <t>Vegetables &amp; mixtures of vegetables othw. than by vinegar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetables, fruit, nuts, fruit-peel &amp; by sugar </t>
+  </si>
+  <si>
+    <t>Homogenised preparations of fruits/nuts, obt. by cooking</t>
+  </si>
+  <si>
+    <t>Edible parts of plants, not containing added sugar</t>
+  </si>
+  <si>
+    <t>Food preparations</t>
+  </si>
+  <si>
+    <t>Waters, incl. mineral waters &amp; aerated waters, containing added sugar</t>
+  </si>
+  <si>
+    <t>Natural honey</t>
+  </si>
+  <si>
+    <t>Peas</t>
+  </si>
+  <si>
+    <t>Olives, provisionally preserved</t>
+  </si>
+  <si>
+    <t>تن ماهی</t>
+  </si>
+  <si>
+    <t>آدامس</t>
+  </si>
+  <si>
+    <t>شکلات</t>
+  </si>
+  <si>
+    <t>کیک</t>
+  </si>
+  <si>
+    <t>ترشی</t>
+  </si>
+  <si>
+    <t>ویفر</t>
+  </si>
+  <si>
+    <t>خیارشور</t>
+  </si>
+  <si>
+    <t>رب گوجه</t>
+  </si>
+  <si>
+    <t>کنسرو سبزیجات</t>
+  </si>
+  <si>
+    <t>کمپوت</t>
+  </si>
+  <si>
+    <t>میوه و آجیل هموژنیزه</t>
+  </si>
+  <si>
+    <t>گیاهان قندی جز شکر</t>
+  </si>
+  <si>
+    <t>آب گازدار</t>
+  </si>
+  <si>
+    <t>کنسرو نخود</t>
+  </si>
+  <si>
+    <t>زیتون</t>
+  </si>
+  <si>
+    <t>شیرینی غیر از آدامس</t>
+  </si>
+  <si>
+    <t>Vegetables &amp; mixtures of vegetables othw. than by vinegar (excl. of 2005.10-2005.91)</t>
+  </si>
+  <si>
+    <t>کنسرو سبزیجات(غیر از 2005.10</t>
+  </si>
+  <si>
+    <t>مواد غذای نیمه آماده</t>
+  </si>
+  <si>
+    <t>p_group</t>
+  </si>
+  <si>
+    <t>E_group</t>
   </si>
 </sst>
 </file>
@@ -242,7 +365,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,11 +388,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,6 +423,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -606,9 +744,11 @@
     <col min="1" max="1" width="22.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -618,10 +758,16 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>56</v>
+      <c r="D1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>16041400</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -629,8 +775,14 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>17041000</v>
       </c>
@@ -640,8 +792,14 @@
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>17049000</v>
       </c>
@@ -651,8 +809,14 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>17049090</v>
       </c>
@@ -662,8 +826,14 @@
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>17049090</v>
       </c>
@@ -673,8 +843,14 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>18069000</v>
       </c>
@@ -684,8 +860,14 @@
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>19041000</v>
       </c>
@@ -695,8 +877,14 @@
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>19053100</v>
       </c>
@@ -706,8 +894,14 @@
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>19053100</v>
       </c>
@@ -717,8 +911,14 @@
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>19053200</v>
       </c>
@@ -728,8 +928,14 @@
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>19059090</v>
       </c>
@@ -739,8 +945,14 @@
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>20011000</v>
       </c>
@@ -750,8 +962,14 @@
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>20019000</v>
       </c>
@@ -761,8 +979,14 @@
       <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>20029010</v>
       </c>
@@ -772,8 +996,14 @@
       <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>20049000</v>
       </c>
@@ -783,8 +1013,14 @@
       <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>20060000</v>
       </c>
@@ -794,8 +1030,14 @@
       <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>20071090</v>
       </c>
@@ -805,8 +1047,14 @@
       <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>20071090</v>
       </c>
@@ -816,8 +1064,14 @@
       <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>20089900</v>
       </c>
@@ -827,8 +1081,14 @@
       <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>21069090</v>
       </c>
@@ -838,8 +1098,14 @@
       <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>22021000</v>
       </c>
@@ -849,8 +1115,14 @@
       <c r="C22" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -860,8 +1132,14 @@
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
@@ -871,8 +1149,14 @@
       <c r="C24" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -882,8 +1166,14 @@
       <c r="C25" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
@@ -893,8 +1183,14 @@
       <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
@@ -902,8 +1198,14 @@
         <v>54</v>
       </c>
       <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -913,8 +1215,14 @@
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
@@ -924,8 +1232,14 @@
       <c r="C29" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>53</v>
       </c>
@@ -935,8 +1249,14 @@
       <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
@@ -946,8 +1266,14 @@
       <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
@@ -957,8 +1283,14 @@
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
@@ -968,8 +1300,14 @@
       <c r="C33" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -979,43 +1317,49 @@
       <c r="C34" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36"/>
       <c r="C36"/>
     </row>
-    <row r="37" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37"/>
       <c r="C37"/>
     </row>
-    <row r="38" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38"/>
       <c r="C38"/>
     </row>
-    <row r="39" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39"/>
       <c r="C39"/>
     </row>
-    <row r="40" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40"/>
       <c r="C40"/>
     </row>
-    <row r="41" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41"/>
       <c r="C41"/>
     </row>
-    <row r="42" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -1038,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1057,7 +1401,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="str">
-        <f>LEFT(A2,6)</f>
+        <f t="shared" ref="B2:B31" si="0">LEFT(A2,6)</f>
         <v>160414</v>
       </c>
     </row>
@@ -1066,7 +1410,7 @@
         <v>17041000</v>
       </c>
       <c r="B3" t="str">
-        <f>LEFT(A3,6)</f>
+        <f t="shared" si="0"/>
         <v>170410</v>
       </c>
     </row>
@@ -1075,7 +1419,7 @@
         <v>17049000</v>
       </c>
       <c r="B4" t="str">
-        <f>LEFT(A4,6)</f>
+        <f t="shared" si="0"/>
         <v>170490</v>
       </c>
     </row>
@@ -1084,7 +1428,7 @@
         <v>17049090</v>
       </c>
       <c r="B5" t="str">
-        <f>LEFT(A5,6)</f>
+        <f t="shared" si="0"/>
         <v>170490</v>
       </c>
     </row>
@@ -1093,7 +1437,7 @@
         <v>18069000</v>
       </c>
       <c r="B6" t="str">
-        <f>LEFT(A6,6)</f>
+        <f t="shared" si="0"/>
         <v>180690</v>
       </c>
     </row>
@@ -1102,7 +1446,7 @@
         <v>19041000</v>
       </c>
       <c r="B7" t="str">
-        <f>LEFT(A7,6)</f>
+        <f t="shared" si="0"/>
         <v>190410</v>
       </c>
     </row>
@@ -1111,7 +1455,7 @@
         <v>19053100</v>
       </c>
       <c r="B8" t="str">
-        <f>LEFT(A8,6)</f>
+        <f t="shared" si="0"/>
         <v>190531</v>
       </c>
     </row>
@@ -1120,7 +1464,7 @@
         <v>19053200</v>
       </c>
       <c r="B9" t="str">
-        <f>LEFT(A9,6)</f>
+        <f t="shared" si="0"/>
         <v>190532</v>
       </c>
     </row>
@@ -1129,7 +1473,7 @@
         <v>19059090</v>
       </c>
       <c r="B10" t="str">
-        <f>LEFT(A10,6)</f>
+        <f t="shared" si="0"/>
         <v>190590</v>
       </c>
     </row>
@@ -1138,7 +1482,7 @@
         <v>20011000</v>
       </c>
       <c r="B11" t="str">
-        <f>LEFT(A11,6)</f>
+        <f t="shared" si="0"/>
         <v>200110</v>
       </c>
     </row>
@@ -1147,7 +1491,7 @@
         <v>20019000</v>
       </c>
       <c r="B12" t="str">
-        <f>LEFT(A12,6)</f>
+        <f t="shared" si="0"/>
         <v>200190</v>
       </c>
     </row>
@@ -1156,7 +1500,7 @@
         <v>20029010</v>
       </c>
       <c r="B13" t="str">
-        <f>LEFT(A13,6)</f>
+        <f t="shared" si="0"/>
         <v>200290</v>
       </c>
     </row>
@@ -1165,7 +1509,7 @@
         <v>20049000</v>
       </c>
       <c r="B14" t="str">
-        <f>LEFT(A14,6)</f>
+        <f t="shared" si="0"/>
         <v>200490</v>
       </c>
     </row>
@@ -1174,7 +1518,7 @@
         <v>20060000</v>
       </c>
       <c r="B15" t="str">
-        <f>LEFT(A15,6)</f>
+        <f t="shared" si="0"/>
         <v>200600</v>
       </c>
     </row>
@@ -1183,7 +1527,7 @@
         <v>20071090</v>
       </c>
       <c r="B16" t="str">
-        <f>LEFT(A16,6)</f>
+        <f t="shared" si="0"/>
         <v>200710</v>
       </c>
     </row>
@@ -1192,7 +1536,7 @@
         <v>20089900</v>
       </c>
       <c r="B17" t="str">
-        <f>LEFT(A17,6)</f>
+        <f t="shared" si="0"/>
         <v>200899</v>
       </c>
     </row>
@@ -1201,7 +1545,7 @@
         <v>21069090</v>
       </c>
       <c r="B18" t="str">
-        <f>LEFT(A18,6)</f>
+        <f t="shared" si="0"/>
         <v>210690</v>
       </c>
     </row>
@@ -1210,7 +1554,7 @@
         <v>22021000</v>
       </c>
       <c r="B19" t="str">
-        <f>LEFT(A19,6)</f>
+        <f t="shared" si="0"/>
         <v>220210</v>
       </c>
     </row>
@@ -1219,7 +1563,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="str">
-        <f>LEFT(A20,6)</f>
+        <f t="shared" si="0"/>
         <v>040900</v>
       </c>
     </row>
@@ -1228,7 +1572,7 @@
         <v>43</v>
       </c>
       <c r="B21" t="str">
-        <f>LEFT(A21,6)</f>
+        <f t="shared" si="0"/>
         <v>071021</v>
       </c>
     </row>
@@ -1237,7 +1581,7 @@
         <v>46</v>
       </c>
       <c r="B22" t="str">
-        <f>LEFT(A22,6)</f>
+        <f t="shared" si="0"/>
         <v>071120</v>
       </c>
     </row>
@@ -1246,7 +1590,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="str">
-        <f>LEFT(A23,6)</f>
+        <f t="shared" si="0"/>
         <v>170490</v>
       </c>
     </row>
@@ -1255,7 +1599,7 @@
         <v>51</v>
       </c>
       <c r="B24" t="str">
-        <f>LEFT(A24,6)</f>
+        <f t="shared" si="0"/>
         <v>170490</v>
       </c>
     </row>
@@ -1264,7 +1608,7 @@
         <v>49</v>
       </c>
       <c r="B25" t="str">
-        <f>LEFT(A25,6)</f>
+        <f t="shared" si="0"/>
         <v>180690</v>
       </c>
     </row>
@@ -1273,7 +1617,7 @@
         <v>33</v>
       </c>
       <c r="B26" t="str">
-        <f>LEFT(A26,6)</f>
+        <f t="shared" si="0"/>
         <v>180690</v>
       </c>
     </row>
@@ -1282,7 +1626,7 @@
         <v>53</v>
       </c>
       <c r="B27" t="str">
-        <f>LEFT(A27,6)</f>
+        <f t="shared" si="0"/>
         <v>190410</v>
       </c>
     </row>
@@ -1291,7 +1635,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="str">
-        <f>LEFT(A28,6)</f>
+        <f t="shared" si="0"/>
         <v>190531</v>
       </c>
     </row>
@@ -1300,7 +1644,7 @@
         <v>52</v>
       </c>
       <c r="B29" t="str">
-        <f>LEFT(A29,6)</f>
+        <f t="shared" si="0"/>
         <v>190532</v>
       </c>
     </row>
@@ -1309,7 +1653,7 @@
         <v>37</v>
       </c>
       <c r="B30" t="str">
-        <f>LEFT(A30,6)</f>
+        <f t="shared" si="0"/>
         <v>200599</v>
       </c>
     </row>
@@ -1318,7 +1662,7 @@
         <v>47</v>
       </c>
       <c r="B31" t="str">
-        <f>LEFT(A31,6)</f>
+        <f t="shared" si="0"/>
         <v>210690</v>
       </c>
     </row>

</xml_diff>